<commit_message>
Update the format of data
</commit_message>
<xml_diff>
--- a/LabelInference/experiment/excel/result.xlsx
+++ b/LabelInference/experiment/excel/result.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linhong\Documents\GitHub\CrossLPTripartite\LabelInference\experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linhong\Documents\GitHub\CrossLPTripartite\LabelInference\experiment\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7680" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="accuracy" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="20">
   <si>
     <t>graph-1</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>difference</t>
+  </si>
+  <si>
+    <t>accuracy</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
@@ -420,6 +423,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -2045,7 +2051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update the accuracy format
</commit_message>
<xml_diff>
--- a/LabelInference/experiment/excel/result.xlsx
+++ b/LabelInference/experiment/excel/result.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="22">
   <si>
     <t>graph-1</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>accuracy</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -409,7 +415,7 @@
   <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V5"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,23 +435,65 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
       <c r="E1" t="s">
         <v>6</v>
       </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
       <c r="K1" t="s">
         <v>8</v>
       </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
       <c r="N1" t="s">
         <v>9</v>
       </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
       <c r="Q1" t="s">
         <v>10</v>
       </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
       <c r="T1" t="s">
         <v>11</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>